<commit_message>
Completed Excel/SQLite conversions and save/load behaviors, including unit tests
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -21,10 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="26">
-  <si>
-    <t>index</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="82">
   <si>
     <t>value</t>
   </si>
@@ -92,13 +89,184 @@
     <t>numberOfCharacters</t>
   </si>
   <si>
-    <t>aggregate</t>
-  </si>
-  <si>
-    <t>error</t>
-  </si>
-  <si>
     <t>isPrime</t>
+  </si>
+  <si>
+    <t>englishName</t>
+  </si>
+  <si>
+    <t>one</t>
+  </si>
+  <si>
+    <t>two</t>
+  </si>
+  <si>
+    <t>three</t>
+  </si>
+  <si>
+    <t>four</t>
+  </si>
+  <si>
+    <t>five</t>
+  </si>
+  <si>
+    <t>six</t>
+  </si>
+  <si>
+    <t>seven</t>
+  </si>
+  <si>
+    <t>eight</t>
+  </si>
+  <si>
+    <t>nine</t>
+  </si>
+  <si>
+    <t>ten</t>
+  </si>
+  <si>
+    <t>eleven</t>
+  </si>
+  <si>
+    <t>twelve</t>
+  </si>
+  <si>
+    <t>thirteen</t>
+  </si>
+  <si>
+    <t>fourteen</t>
+  </si>
+  <si>
+    <t>fifteen</t>
+  </si>
+  <si>
+    <t>sixteen</t>
+  </si>
+  <si>
+    <t>seventeen</t>
+  </si>
+  <si>
+    <t>eighteen</t>
+  </si>
+  <si>
+    <t>nineteen</t>
+  </si>
+  <si>
+    <t>twenty</t>
+  </si>
+  <si>
+    <t>twenty-one</t>
+  </si>
+  <si>
+    <t>twenty-two</t>
+  </si>
+  <si>
+    <t>twenty-three</t>
+  </si>
+  <si>
+    <t>twenty-four</t>
+  </si>
+  <si>
+    <t>twenty-five</t>
+  </si>
+  <si>
+    <t>twenty-six</t>
+  </si>
+  <si>
+    <t>twenty-seven</t>
+  </si>
+  <si>
+    <t>twenty-eight</t>
+  </si>
+  <si>
+    <t>twenty-nine</t>
+  </si>
+  <si>
+    <t>thirty</t>
+  </si>
+  <si>
+    <t>fourty</t>
+  </si>
+  <si>
+    <t>fourty-three</t>
+  </si>
+  <si>
+    <t>thirty-one</t>
+  </si>
+  <si>
+    <t>thirty-two</t>
+  </si>
+  <si>
+    <t>thirty-three</t>
+  </si>
+  <si>
+    <t>thirty-four</t>
+  </si>
+  <si>
+    <t>thirty-five</t>
+  </si>
+  <si>
+    <t>thirty-six</t>
+  </si>
+  <si>
+    <t>thirty-seven</t>
+  </si>
+  <si>
+    <t>thirty-eight</t>
+  </si>
+  <si>
+    <t>thirty-nine</t>
+  </si>
+  <si>
+    <t>fourty-one</t>
+  </si>
+  <si>
+    <t>fourty-two</t>
+  </si>
+  <si>
+    <t>ndx</t>
+  </si>
+  <si>
+    <t>f2</t>
+  </si>
+  <si>
+    <t>f3</t>
+  </si>
+  <si>
+    <t>f5</t>
+  </si>
+  <si>
+    <t>f7</t>
+  </si>
+  <si>
+    <t>f11</t>
+  </si>
+  <si>
+    <t>f13</t>
+  </si>
+  <si>
+    <t>f17</t>
+  </si>
+  <si>
+    <t>f19</t>
+  </si>
+  <si>
+    <t>f23</t>
+  </si>
+  <si>
+    <t>f29</t>
+  </si>
+  <si>
+    <t>f31</t>
+  </si>
+  <si>
+    <t>f37</t>
+  </si>
+  <si>
+    <t>f41</t>
+  </si>
+  <si>
+    <t>f43</t>
   </si>
 </sst>
 </file>
@@ -463,25 +631,25 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C30" sqref="A1:C32"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -492,7 +660,7 @@
         <v>3.2601788152152258</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -504,7 +672,7 @@
         <v>3.6901688505230448</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -516,7 +684,7 @@
         <v>6.7979190226481379</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -528,7 +696,7 @@
         <v>7.8293885646846899</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -540,7 +708,7 @@
         <v>8.9849333527419937</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -552,7 +720,7 @@
         <v>7.3143647186495491</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -564,7 +732,7 @@
         <v>12.739762236259867</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -576,7 +744,7 @@
         <v>9.5672083430408001</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -588,7 +756,7 @@
         <v>15.004405279698133</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -600,7 +768,7 @@
         <v>13.489262017880176</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -612,7 +780,7 @@
         <v>21.013886590029824</v>
       </c>
       <c r="C12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -624,7 +792,7 @@
         <v>24.165987987815569</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -636,7 +804,7 @@
         <v>21.581812139300556</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -648,7 +816,7 @@
         <v>20.13249207150162</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -660,7 +828,7 @@
         <v>16.37265479267036</v>
       </c>
       <c r="C16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -672,7 +840,7 @@
         <v>21.879717011227775</v>
       </c>
       <c r="C17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -684,7 +852,7 @@
         <v>20.388384273660037</v>
       </c>
       <c r="C18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -696,7 +864,7 @@
         <v>27.704900839769472</v>
       </c>
       <c r="C19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -708,7 +876,7 @@
         <v>21.459389373377928</v>
       </c>
       <c r="C20" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -720,7 +888,7 @@
         <v>39.401252525809006</v>
       </c>
       <c r="C21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -732,7 +900,7 @@
         <v>42.746333686417515</v>
       </c>
       <c r="C22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -744,7 +912,7 @@
         <v>33.795588667735629</v>
       </c>
       <c r="C23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -756,7 +924,7 @@
         <v>36.531398158754904</v>
       </c>
       <c r="C24" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -768,7 +936,7 @@
         <v>41.708223977792812</v>
       </c>
       <c r="C25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -780,7 +948,7 @@
         <v>49.30167390843112</v>
       </c>
       <c r="C26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -792,7 +960,7 @@
         <v>52.350694789461485</v>
       </c>
       <c r="C27" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -804,7 +972,7 @@
         <v>47.932243548111245</v>
       </c>
       <c r="C28" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -816,7 +984,7 @@
         <v>40.749478672616647</v>
       </c>
       <c r="C29" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -828,7 +996,7 @@
         <v>32.794811445828643</v>
       </c>
       <c r="C30" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -840,7 +1008,7 @@
         <v>40.509165818544176</v>
       </c>
       <c r="C31" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -852,7 +1020,7 @@
         <v>52.957848997962088</v>
       </c>
       <c r="C32" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -863,139 +1031,130 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R44"/>
+  <dimension ref="A1:Q44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L11" sqref="L11"/>
+      <selection pane="bottomLeft" activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="2.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="15" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="15" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1">
-        <v>7</v>
-      </c>
-      <c r="F1" s="1">
-        <v>11</v>
-      </c>
-      <c r="G1" s="1">
-        <v>13</v>
-      </c>
-      <c r="H1" s="1">
-        <v>17</v>
-      </c>
-      <c r="I1" s="1">
-        <v>19</v>
-      </c>
-      <c r="J1" s="1">
+        <v>67</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="1">
-        <v>29</v>
-      </c>
-      <c r="L1" s="1">
-        <v>31</v>
-      </c>
-      <c r="M1" s="1">
-        <v>37</v>
-      </c>
-      <c r="N1" s="1">
-        <v>41</v>
-      </c>
-      <c r="O1" s="1">
-        <v>43</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2" t="b">
+        <f>SUM(B2:O2)=1</f>
+        <v>0</v>
+      </c>
+      <c r="Q2" t="s">
         <v>24</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <f>POWER($B$1,B2)*POWER($C$1,C2)*POWER($D$1,D2)*POWER($E$1,E2)*POWER($F$1,F2)*POWER($G$1,G2)*POWER($H$1,H2)*POWER($I$1,I2)*POWER($J$1,J2)*POWER($K$1,K2)*POWER($L$1,L2)*POWER($M$1,M2)*POWER($N$1,N2)*POWER($O$1,O2)</f>
-        <v>1</v>
-      </c>
-      <c r="Q2">
-        <f>P2-A2</f>
-        <v>0</v>
-      </c>
-      <c r="R2" t="b">
-        <f>SUM(B2:O2)=1</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -1042,22 +1201,17 @@
       <c r="O3">
         <v>0</v>
       </c>
-      <c r="P3">
-        <f t="shared" ref="P3:P44" si="0">POWER($B$1,B3)*POWER($C$1,C3)*POWER($D$1,D3)*POWER($E$1,E3)*POWER($F$1,F3)*POWER($G$1,G3)*POWER($H$1,H3)*POWER($I$1,I3)*POWER($J$1,J3)*POWER($K$1,K3)*POWER($L$1,L3)*POWER($M$1,M3)*POWER($N$1,N3)*POWER($O$1,O3)</f>
-        <v>2</v>
-      </c>
-      <c r="Q3">
-        <f t="shared" ref="Q3:Q44" si="1">P3-A3</f>
-        <v>0</v>
-      </c>
-      <c r="R3" t="b">
-        <f t="shared" ref="R3:R44" si="2">SUM(B3:O3)=1</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P3" t="b">
+        <f t="shared" ref="P3:P44" si="0">SUM(B3:O3)=1</f>
+        <v>1</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A44" si="3">A3+1</f>
+        <f t="shared" ref="A4:A44" si="1">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4">
@@ -1102,22 +1256,17 @@
       <c r="O4">
         <v>0</v>
       </c>
-      <c r="P4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="Q4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R4" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P4" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="B5">
@@ -1162,22 +1311,17 @@
       <c r="O5">
         <v>0</v>
       </c>
-      <c r="P5">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="Q5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R5" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P5" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B6">
@@ -1222,22 +1366,17 @@
       <c r="O6">
         <v>0</v>
       </c>
-      <c r="P6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="Q6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R6" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P6" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B7">
@@ -1282,22 +1421,17 @@
       <c r="O7">
         <v>0</v>
       </c>
-      <c r="P7">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="Q7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R7" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P7" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B8">
@@ -1342,22 +1476,17 @@
       <c r="O8">
         <v>0</v>
       </c>
-      <c r="P8">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="Q8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R8" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P8" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B9">
@@ -1402,22 +1531,17 @@
       <c r="O9">
         <v>0</v>
       </c>
-      <c r="P9">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="Q9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R9" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P9" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B10">
@@ -1462,22 +1586,17 @@
       <c r="O10">
         <v>0</v>
       </c>
-      <c r="P10">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="Q10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R10" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P10" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B11">
@@ -1522,22 +1641,17 @@
       <c r="O11">
         <v>0</v>
       </c>
-      <c r="P11">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="Q11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R11" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P11" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="B12">
@@ -1582,22 +1696,17 @@
       <c r="O12">
         <v>0</v>
       </c>
-      <c r="P12">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="Q12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R12" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B13">
@@ -1642,22 +1751,17 @@
       <c r="O13">
         <v>0</v>
       </c>
-      <c r="P13">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="Q13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R13" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P13" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B14">
@@ -1702,22 +1806,17 @@
       <c r="O14">
         <v>0</v>
       </c>
-      <c r="P14">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="Q14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R14" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P14" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="B15">
@@ -1762,22 +1861,17 @@
       <c r="O15">
         <v>0</v>
       </c>
-      <c r="P15">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="Q15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R15" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P15" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B16">
@@ -1822,22 +1916,17 @@
       <c r="O16">
         <v>0</v>
       </c>
-      <c r="P16">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="Q16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R16" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P16" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="B17">
@@ -1882,22 +1971,17 @@
       <c r="O17">
         <v>0</v>
       </c>
-      <c r="P17">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="Q17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R17" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P17" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="B18">
@@ -1942,22 +2026,17 @@
       <c r="O18">
         <v>0</v>
       </c>
-      <c r="P18">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="Q18">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R18" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P18" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="B19">
@@ -2002,22 +2081,17 @@
       <c r="O19">
         <v>0</v>
       </c>
-      <c r="P19">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="Q19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R19" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P19" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="B20">
@@ -2062,22 +2136,17 @@
       <c r="O20">
         <v>0</v>
       </c>
-      <c r="P20">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="Q20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R20" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P20" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="B21">
@@ -2122,22 +2191,17 @@
       <c r="O21">
         <v>0</v>
       </c>
-      <c r="P21">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="Q21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R21" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P21" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="B22">
@@ -2182,22 +2246,17 @@
       <c r="O22">
         <v>0</v>
       </c>
-      <c r="P22">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="Q22">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R22" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P22" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="B23">
@@ -2242,22 +2301,17 @@
       <c r="O23">
         <v>0</v>
       </c>
-      <c r="P23">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="Q23">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R23" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P23" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="B24">
@@ -2302,22 +2356,17 @@
       <c r="O24">
         <v>0</v>
       </c>
-      <c r="P24">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="Q24">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R24" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P24" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="B25">
@@ -2362,22 +2411,17 @@
       <c r="O25">
         <v>0</v>
       </c>
-      <c r="P25">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="Q25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R25" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P25" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="B26">
@@ -2422,22 +2466,17 @@
       <c r="O26">
         <v>0</v>
       </c>
-      <c r="P26">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="Q26">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R26" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P26" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="B27">
@@ -2482,22 +2521,17 @@
       <c r="O27">
         <v>0</v>
       </c>
-      <c r="P27">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="Q27">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R27" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P27" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="B28">
@@ -2542,22 +2576,17 @@
       <c r="O28">
         <v>0</v>
       </c>
-      <c r="P28">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="Q28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R28" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P28" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="B29">
@@ -2602,22 +2631,17 @@
       <c r="O29">
         <v>0</v>
       </c>
-      <c r="P29">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="Q29">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R29" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P29" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="B30">
@@ -2662,22 +2686,17 @@
       <c r="O30">
         <v>0</v>
       </c>
-      <c r="P30">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="Q30">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R30" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P30" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="B31">
@@ -2722,22 +2741,17 @@
       <c r="O31">
         <v>0</v>
       </c>
-      <c r="P31">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="Q31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R31" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P31" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="B32">
@@ -2782,22 +2796,17 @@
       <c r="O32">
         <v>0</v>
       </c>
-      <c r="P32">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="Q32">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R32" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P32" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="B33">
@@ -2842,22 +2851,17 @@
       <c r="O33">
         <v>0</v>
       </c>
-      <c r="P33">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="Q33">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R33" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P33" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="B34">
@@ -2902,22 +2906,17 @@
       <c r="O34">
         <v>0</v>
       </c>
-      <c r="P34">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="Q34">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R34" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P34" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="B35">
@@ -2962,22 +2961,17 @@
       <c r="O35">
         <v>0</v>
       </c>
-      <c r="P35">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="Q35">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R35" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P35" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="B36">
@@ -3022,22 +3016,17 @@
       <c r="O36">
         <v>0</v>
       </c>
-      <c r="P36">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="Q36">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R36" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P36" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="B37">
@@ -3082,22 +3071,17 @@
       <c r="O37">
         <v>0</v>
       </c>
-      <c r="P37">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="Q37">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R37" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P37" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="B38">
@@ -3142,22 +3126,17 @@
       <c r="O38">
         <v>0</v>
       </c>
-      <c r="P38">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-      <c r="Q38">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R38" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P38" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="B39">
@@ -3202,22 +3181,17 @@
       <c r="O39">
         <v>0</v>
       </c>
-      <c r="P39">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="Q39">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R39" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P39" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="B40">
@@ -3262,22 +3236,17 @@
       <c r="O40">
         <v>0</v>
       </c>
-      <c r="P40">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-      <c r="Q40">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R40" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P40" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="B41">
@@ -3322,22 +3291,17 @@
       <c r="O41">
         <v>0</v>
       </c>
-      <c r="P41">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="Q41">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R41" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P41" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="B42">
@@ -3382,22 +3346,17 @@
       <c r="O42">
         <v>0</v>
       </c>
-      <c r="P42">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="Q42">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R42" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P42" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="B43">
@@ -3442,22 +3401,17 @@
       <c r="O43">
         <v>0</v>
       </c>
-      <c r="P43">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="Q43">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R43" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P43" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="B44">
@@ -3502,17 +3456,12 @@
       <c r="O44">
         <v>1</v>
       </c>
-      <c r="P44">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="Q44">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R44" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
+      <c r="P44" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -3526,24 +3475,25 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3551,7 +3501,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2">
         <f>LEN(B2)</f>
@@ -3564,7 +3514,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C16" si="0">LEN(B3)</f>
@@ -3577,7 +3527,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
@@ -3590,7 +3540,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
@@ -3603,7 +3553,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
@@ -3616,7 +3566,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
@@ -3629,7 +3579,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
@@ -3642,7 +3592,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
@@ -3655,7 +3605,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
@@ -3668,7 +3618,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
@@ -3681,7 +3631,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
@@ -3694,7 +3644,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
@@ -3707,7 +3657,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
@@ -3720,7 +3670,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
@@ -3733,7 +3683,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>

</xml_diff>